<commit_message>
Listo ajustes front, empezando a crear API Acceso a Datos
</commit_message>
<xml_diff>
--- a/Archivos/Estructura BD.xlsx
+++ b/Archivos/Estructura BD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\Andes Tool\Registro Incidentes Bomberos\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D65F38-ABEF-4D9F-8347-A23754B24775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B86B6BB-3B74-4B30-AA96-98DCC289713F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
   <si>
     <t>Usuarios</t>
   </si>
@@ -54,9 +54,6 @@
     <t>TipoSiniestro</t>
   </si>
   <si>
-    <t>Comuna/Region</t>
-  </si>
-  <si>
     <t>Conductores</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Relato</t>
   </si>
   <si>
-    <t>DañosVehiculoAsegurado</t>
-  </si>
-  <si>
     <t>NumeroPartePolicial</t>
   </si>
   <si>
@@ -174,17 +168,71 @@
     <t>FechaHora</t>
   </si>
   <si>
-    <t>Comentario</t>
-  </si>
-  <si>
     <t>LiquidadorACargo (¿Normalizado?) | ¿Es usuario de Seguros?</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>TiposConductores</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>DaniosVehiculoAsegurado</t>
+  </si>
+  <si>
+    <t>Regiones</t>
+  </si>
+  <si>
+    <t>Ciudades</t>
+  </si>
+  <si>
+    <t>Comisarias</t>
+  </si>
+  <si>
+    <t>IdRegion</t>
+  </si>
+  <si>
+    <t>MarcasVehiculos</t>
+  </si>
+  <si>
+    <t>ModelosVehiculos</t>
+  </si>
+  <si>
+    <t>IdMarca</t>
+  </si>
+  <si>
+    <t>Talleres</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>Estados</t>
+  </si>
+  <si>
+    <t>IdUsuario</t>
+  </si>
+  <si>
+    <t>MarcasChasis</t>
+  </si>
+  <si>
+    <t>ModelosChasis</t>
+  </si>
+  <si>
+    <t>TiposPadrones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +248,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,8 +269,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -309,25 +369,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,9 +680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F24"/>
+  <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -618,224 +694,333 @@
     <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.109375" customWidth="1"/>
     <col min="6" max="6" width="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
-        <v>41</v>
+        <v>29</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F10" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="J10" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="7" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="11" t="s">
-        <v>41</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D21" s="10" t="s">
+    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D23" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="8" t="s">
-        <v>45</v>
+      <c r="H25" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H26" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H27" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Termine de configurar los ambientes, arrancando a reconocer usuario en Front
</commit_message>
<xml_diff>
--- a/Archivos/Estructura BD.xlsx
+++ b/Archivos/Estructura BD.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\Andes Tool\Registro Incidentes Bomberos\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B86B6BB-3B74-4B30-AA96-98DCC289713F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E12691-8C1D-4395-98B7-30D63591AF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>Usuarios</t>
   </si>
@@ -226,6 +237,18 @@
   </si>
   <si>
     <t>TiposPadrones</t>
+  </si>
+  <si>
+    <t>Comisaria</t>
+  </si>
+  <si>
+    <t>TercerosInvolucrados (Si/No)</t>
+  </si>
+  <si>
+    <t>CuerposBomberos</t>
+  </si>
+  <si>
+    <t>&lt;--- Seguro tiene otros datos</t>
   </si>
 </sst>
 </file>
@@ -275,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -382,12 +405,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -399,6 +435,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -680,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J27"/>
+  <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,7 +734,7 @@
     <col min="7" max="7" width="3.33203125" customWidth="1"/>
     <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -858,7 +895,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>36</v>
@@ -872,7 +909,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>37</v>
@@ -886,7 +923,7 @@
         <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>54</v>
@@ -900,7 +937,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>38</v>
@@ -917,7 +954,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>40</v>
@@ -926,20 +963,20 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J17" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>44</v>
@@ -951,9 +988,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D19" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>45</v>
@@ -962,9 +999,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>43</v>
@@ -972,18 +1009,27 @@
       <c r="H20" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J20" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D22" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>63</v>
@@ -992,33 +1038,39 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="H25" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D26" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="H26" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H27" s="2" t="s">
         <v>59</v>
       </c>

</xml_diff>